<commit_message>
Updated Chart due to an error in the previous one
</commit_message>
<xml_diff>
--- a/burndown chart.xlsx
+++ b/burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teodoroadinolfi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graziaferrara/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A74C91-EEB3-E24A-B34D-FF59B15B33C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF7629A-5FC4-7F4B-AD11-1B1A84BF06AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{26103C1A-F694-E24A-ADA3-F68FE605EF20}"/>
+    <workbookView xWindow="34700" yWindow="3260" windowWidth="28800" windowHeight="16360" xr2:uid="{26103C1A-F694-E24A-ADA3-F68FE605EF20}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="4" r:id="rId1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -414,7 +411,7 @@
                   <c:v>274</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>205</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2D51F4-7E60-094A-AEDC-138C5ED9BA8E}">
   <dimension ref="B2:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1001,7 +998,7 @@
         <v>274</v>
       </c>
       <c r="F3" s="4">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -1019,7 +1016,7 @@
       </c>
       <c r="E4" s="4">
         <f>E3-F3</f>
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
Upload of the last version of the burndown chart
</commit_message>
<xml_diff>
--- a/burndown chart.xlsx
+++ b/burndown chart.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graziaferrara/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF7629A-5FC4-7F4B-AD11-1B1A84BF06AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19086D42-EA8E-4544-9129-5ECA213E62C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34700" yWindow="3260" windowWidth="28800" windowHeight="16360" xr2:uid="{26103C1A-F694-E24A-ADA3-F68FE605EF20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{26103C1A-F694-E24A-ADA3-F68FE605EF20}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -333,6 +336,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -412,6 +421,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -951,19 +963,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2D51F4-7E60-094A-AEDC-138C5ED9BA8E}">
   <dimension ref="B2:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.875" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.625" customWidth="1"/>
     <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -983,7 +995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1000,9 +1012,11 @@
       <c r="F3" s="4">
         <v>77</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1019,11 +1033,13 @@
         <v>197</v>
       </c>
       <c r="F4" s="4">
+        <v>76</v>
+      </c>
+      <c r="G4" s="4">
         <v>0</v>
       </c>
-      <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1035,11 +1051,14 @@
         <f>C5-C6</f>
         <v>92</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4">
+        <f>E4-F4</f>
+        <v>121</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1055,7 +1074,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
   </sheetData>

</xml_diff>